<commit_message>
Finalisation analyse, Création projet android studio
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail_VMW.xlsx
+++ b/Documentation/Journal_de_travail_VMW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt63nch\Documents\GitHub\Oublie pas\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BB0F64-B9E8-4AD2-9D5B-1A9E76908969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA04714C-1AB0-4C5A-AE98-EEE61D1FA1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11340" yWindow="6345" windowWidth="21600" windowHeight="11385" xr2:uid="{C76477CB-AF63-4402-801C-627B6AD4564C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C76477CB-AF63-4402-801C-627B6AD4564C}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Finalisation de ma planification initiale</t>
   </si>
   <si>
-    <t>Cristalle Kendra Guissaz</t>
-  </si>
-  <si>
     <t>Ayant pris beaucoup de retard avec l'application j'ai demandé de l'aide a ma collegue Cristalle kendra Guissaz et pu finir dans les temps</t>
   </si>
   <si>
@@ -139,16 +136,53 @@
   </si>
   <si>
     <t>Journal de travail et mise a jour de documentation</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Mise a jour du journal de travail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Dossier de conception dans le Dossier de projet</t>
+  </si>
+  <si>
+    <t>Mise a jour des image dans le dossier de projet</t>
+  </si>
+  <si>
+    <t>Correction de diverse faute d'orthographe et grammaire</t>
+  </si>
+  <si>
+    <t>Cristalle Kendra Gueissaz</t>
+  </si>
+  <si>
+    <t>Strategie de test</t>
+  </si>
+  <si>
+    <t>Modification maquette et diagramme de flux</t>
+  </si>
+  <si>
+    <t>Création du projet sur Android studio</t>
+  </si>
+  <si>
+    <t>Planification du projet Sur Github</t>
+  </si>
+  <si>
+    <t>Finalisation d'analyse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="[h]:mm:ss\ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,13 +197,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -195,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -219,11 +278,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -266,16 +331,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}" name="Tableau1" displayName="Tableau1" ref="A1:G37" totalsRowShown="0" dataDxfId="7">
-  <autoFilter ref="A1:G37" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F03BD8AE-DCAD-435E-AC03-584E15FC8493}" name="Date" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{76FA6963-7F8C-4895-B8BA-445A4BB2DC8E}" name="Type de travail" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{C9139E1C-787D-4C5A-8750-6FE082AAC00C}" name="Description" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{B117813D-6F0A-4286-980F-99C6DC102ADB}" name="Problème rencontré / remarque" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{C96D9B9A-7860-4266-842C-6C83AAF6F623}" name="heure de début2" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{8CEFA920-E3F0-445D-B615-5599E28C54E8}" name="Heure de fin" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{6318CDEB-0B8E-473F-94F7-20D613FF13AB}" name="Intervenant" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}" name="Tableau1" displayName="Tableau1" ref="A1:H36" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="A1:H36" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{F03BD8AE-DCAD-435E-AC03-584E15FC8493}" name="Date" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{76FA6963-7F8C-4895-B8BA-445A4BB2DC8E}" name="Type de travail" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{C9139E1C-787D-4C5A-8750-6FE082AAC00C}" name="Description" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{B117813D-6F0A-4286-980F-99C6DC102ADB}" name="Problème rencontré / remarque" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{C96D9B9A-7860-4266-842C-6C83AAF6F623}" name="heure de début2" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{8CEFA920-E3F0-445D-B615-5599E28C54E8}" name="Heure de fin" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{90F7EFB8-458C-4FFB-857D-6CD3E697FB07}" name="Total" dataDxfId="0">
+      <calculatedColumnFormula>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{6318CDEB-0B8E-473F-94F7-20D613FF13AB}" name="Intervenant" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -578,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4812EB-3ED2-43D9-9F10-833A2D245EB4}">
-  <dimension ref="A1:G115"/>
+  <dimension ref="A1:I114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,10 +660,11 @@
     <col min="4" max="4" width="53.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="93.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -614,11 +683,17 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>45412</v>
       </c>
@@ -626,7 +701,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="7">
@@ -635,9 +710,17 @@
       <c r="F2" s="7">
         <v>0.35416666666666669</v>
       </c>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="10">
+        <f>SUM(G:G)</f>
+        <v>1.2222222222222219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>45412</v>
       </c>
@@ -651,14 +734,18 @@
         <v>8</v>
       </c>
       <c r="E3" s="7">
-        <v>0.375</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="F3" s="7">
         <v>0.39930555555555558</v>
       </c>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G3" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>4.5138888888888895E-2</v>
+      </c>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>45412</v>
       </c>
@@ -672,14 +759,18 @@
         <v>12</v>
       </c>
       <c r="E4" s="7">
-        <v>0.375</v>
+        <v>0.40972222222222227</v>
       </c>
       <c r="F4" s="7">
         <v>0.41666666666666669</v>
       </c>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G4" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>45412</v>
       </c>
@@ -698,9 +789,13 @@
       <c r="F5" s="7">
         <v>0.51041666666666663</v>
       </c>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G5" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>9.3749999999999944E-2</v>
+      </c>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>45412</v>
       </c>
@@ -708,7 +803,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="7">
@@ -717,9 +812,13 @@
       <c r="F6" s="7">
         <v>0.64583333333333337</v>
       </c>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="G6" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>45412</v>
       </c>
@@ -730,7 +829,7 @@
         <v>16</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="7">
         <v>0.64583333333333337</v>
@@ -738,11 +837,15 @@
       <c r="F7" s="7">
         <v>0.70138888888888884</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>5.5555555555555469E-2</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>45414</v>
       </c>
@@ -759,9 +862,13 @@
       <c r="F8" s="7">
         <v>0.39930555555555558</v>
       </c>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G8" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>45414</v>
       </c>
@@ -772,7 +879,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="7">
         <v>0.40972222222222227</v>
@@ -780,9 +887,13 @@
       <c r="F9" s="7">
         <v>0.4375</v>
       </c>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>2.7777777777777735E-2</v>
+      </c>
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>45414</v>
       </c>
@@ -790,7 +901,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="7">
@@ -799,9 +910,13 @@
       <c r="F10" s="7">
         <v>0.46875</v>
       </c>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G10" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>45414</v>
       </c>
@@ -809,7 +924,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="7">
@@ -818,9 +933,13 @@
       <c r="F11" s="7">
         <v>0.49305555555555558</v>
       </c>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>45415</v>
       </c>
@@ -828,20 +947,24 @@
         <v>5</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="7">
-        <v>0.34722222222222227</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F12" s="7">
         <v>0.39930555555555558</v>
       </c>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>6.5972222222222265E-2</v>
+      </c>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>45415</v>
       </c>
@@ -849,10 +972,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>25</v>
       </c>
       <c r="E13" s="7">
         <v>0.40972222222222227</v>
@@ -860,9 +983,13 @@
       <c r="F13" s="7">
         <v>0.43055555555555558</v>
       </c>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>45415</v>
       </c>
@@ -870,10 +997,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="7">
         <v>0.43055555555555558</v>
@@ -881,9 +1008,13 @@
       <c r="F14" s="7">
         <v>0.46527777777777773</v>
       </c>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G14" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>3.4722222222222154E-2</v>
+      </c>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>45415</v>
       </c>
@@ -891,20 +1022,24 @@
         <v>5</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" s="7">
-        <v>0.43055555555555558</v>
+        <v>0.46527777777777773</v>
       </c>
       <c r="F15" s="7">
         <v>0.49305555555555558</v>
       </c>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>2.7777777777777846E-2</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>45415</v>
       </c>
@@ -912,7 +1047,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="7">
@@ -921,9 +1056,13 @@
       <c r="F16" s="7">
         <v>0.51041666666666663</v>
       </c>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G16" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>45415</v>
       </c>
@@ -931,7 +1070,7 @@
         <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="7">
@@ -940,9 +1079,13 @@
       <c r="F17" s="7">
         <v>0.59375</v>
       </c>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>45415</v>
       </c>
@@ -950,7 +1093,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="7">
@@ -959,9 +1102,13 @@
       <c r="F18" s="7">
         <v>0.61458333333333337</v>
       </c>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>45415</v>
       </c>
@@ -969,10 +1116,10 @@
         <v>15</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="E19" s="7">
         <v>0.61458333333333337</v>
@@ -980,9 +1127,13 @@
       <c r="F19" s="7">
         <v>0.69791666666666663</v>
       </c>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G19" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>8.3333333333333259E-2</v>
+      </c>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>45415</v>
       </c>
@@ -990,7 +1141,7 @@
         <v>15</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="7">
@@ -999,202 +1150,344 @@
       <c r="F20" s="7">
         <v>0.70486111111111116</v>
       </c>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="5"/>
+      <c r="G20" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>6.9444444444445308E-3</v>
+      </c>
+      <c r="H20" s="7"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>45418</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5"/>
+      <c r="E21" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="G21" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>6.5972222222222265E-2</v>
+      </c>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>45418</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="D22" s="6"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
+      <c r="E22" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="G22" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>0.10069444444444436</v>
+      </c>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>45418</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="G23" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="H23" s="7"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>45418</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5"/>
+      <c r="E24" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="G24" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>6.5972222222222265E-2</v>
+      </c>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>45419</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="D25" s="6"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
+      <c r="E25" s="7">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="8"/>
+      <c r="H25" s="7"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>45419</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="D26" s="6"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="5"/>
+      <c r="E26" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F26" s="7">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="G26" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>5.2083333333333315E-2</v>
+      </c>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>45419</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="D27" s="6"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="5"/>
+      <c r="E27" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="F27" s="7">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="G27" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>45419</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="D28" s="6"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="7">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="G28" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>7.6388888888888951E-2</v>
+      </c>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="7"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="7"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="7"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
@@ -1462,11 +1755,8 @@
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C115" s="2"/>
-      <c r="D115" s="2"/>
-    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="80" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
@@ -1476,12 +1766,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1599,15 +1886,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC60CD4A-9E4F-42F0-BE26-5B273C83DB90}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{213C64E1-87E2-4C8E-8457-B15D2DEDA5D9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1629,16 +1926,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{213C64E1-87E2-4C8E-8457-B15D2DEDA5D9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC60CD4A-9E4F-42F0-BE26-5B273C83DB90}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Création d'un projet de test
Afin d'avoir un environnement simple pour tester l'ajout de divers classes et fonctions, ce projet pour expérimenter de nouvelles fonctions a été ajouté au projet.
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail_VMW.xlsx
+++ b/Documentation/Journal_de_travail_VMW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt63nch\Documents\GitHub\Oublie pas\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA04714C-1AB0-4C5A-AE98-EEE61D1FA1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADE72D4-9C25-4B27-9B90-90F52F712B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C76477CB-AF63-4402-801C-627B6AD4564C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="70">
   <si>
     <t>Date</t>
   </si>
@@ -172,6 +172,78 @@
   </si>
   <si>
     <t>Finalisation d'analyse</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Recommencé le projet avec la bonne template.</t>
+  </si>
+  <si>
+    <t>Ajouts des layouts de la main page et de mainobjectif.</t>
+  </si>
+  <si>
+    <t>Création de layout pour les item des recycleur.</t>
+  </si>
+  <si>
+    <t>Creations des derniers layouts, modifier et paramètres</t>
+  </si>
+  <si>
+    <t>Ajout de classes respective de chaque activité.</t>
+  </si>
+  <si>
+    <t>Mise a jour de l'androidManifest en conséquence</t>
+  </si>
+  <si>
+    <t>Implementation de la classe NavigationHandler</t>
+  </si>
+  <si>
+    <t>Je n'aurais normalement plus besoin de toucher les mouvement ou la classe navigation handler</t>
+  </si>
+  <si>
+    <t>Création de toutes les fonctions necessaire</t>
+  </si>
+  <si>
+    <t>Nettoyage du code</t>
+  </si>
+  <si>
+    <t>Amelioration de la lisibilité globale du projet.</t>
+  </si>
+  <si>
+    <t>Création du recyclerAdapter</t>
+  </si>
+  <si>
+    <t>Pour le menu principal</t>
+  </si>
+  <si>
+    <t>Pour les catégories custom</t>
+  </si>
+  <si>
+    <t>Création du recyclerAdapterCategorie</t>
+  </si>
+  <si>
+    <t>finition de la navigation pour chaque layout</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Journal de travail</t>
+  </si>
+  <si>
+    <t>Documentation de l'implementation effectué jusqu’à maintenant.</t>
+  </si>
+  <si>
+    <t>Débogage</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> j'avais un bug avec une erreur humaine dans les noms choisi pour les ID de mes elements dans mes layouts et cela fesait crash mon application</t>
+  </si>
+  <si>
+    <t>entretien expert</t>
+  </si>
+  <si>
+    <t>monsieur Ferrari</t>
   </si>
 </sst>
 </file>
@@ -180,7 +252,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="[h]:mm:ss\ "/>
+    <numFmt numFmtId="165" formatCode="[h]:mm:ss\ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -279,7 +351,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -287,11 +359,11 @@
   <dxfs count="9">
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -331,8 +403,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}" name="Tableau1" displayName="Tableau1" ref="A1:H36" totalsRowShown="0" dataDxfId="8">
-  <autoFilter ref="A1:H36" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}" name="Tableau1" displayName="Tableau1" ref="A1:H44" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="A1:H44" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F03BD8AE-DCAD-435E-AC03-584E15FC8493}" name="Date" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{76FA6963-7F8C-4895-B8BA-445A4BB2DC8E}" name="Type de travail" dataDxfId="6"/>
@@ -340,10 +412,10 @@
     <tableColumn id="4" xr3:uid="{B117813D-6F0A-4286-980F-99C6DC102ADB}" name="Problème rencontré / remarque" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{C96D9B9A-7860-4266-842C-6C83AAF6F623}" name="heure de début2" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{8CEFA920-E3F0-445D-B615-5599E28C54E8}" name="Heure de fin" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{90F7EFB8-458C-4FFB-857D-6CD3E697FB07}" name="Total" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{90F7EFB8-458C-4FFB-857D-6CD3E697FB07}" name="Total" dataDxfId="1">
       <calculatedColumnFormula>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6318CDEB-0B8E-473F-94F7-20D613FF13AB}" name="Intervenant" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{6318CDEB-0B8E-473F-94F7-20D613FF13AB}" name="Intervenant" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -648,15 +720,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4812EB-3ED2-43D9-9F10-833A2D245EB4}">
   <dimension ref="A1:I114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="46.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -717,7 +789,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="10">
         <f>SUM(G:G)</f>
-        <v>1.2222222222222219</v>
+        <v>1.725694444444444</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1179,7 +1251,7 @@
       </c>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>45418</v>
       </c>
@@ -1267,7 +1339,10 @@
       <c r="F25" s="7">
         <v>0.45833333333333331</v>
       </c>
-      <c r="G25" s="7"/>
+      <c r="G25" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>5.9027777777777735E-2</v>
+      </c>
       <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1298,7 +1373,7 @@
         <v>45419</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>43</v>
@@ -1340,140 +1415,384 @@
       <c r="H28" s="7"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="5"/>
+      <c r="A29" s="3">
+        <v>45425</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="D29" s="6"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
+      <c r="E29" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0.35416666666666669</v>
+      </c>
       <c r="G29" s="7">
         <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="5"/>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>45425</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
+      <c r="E30" s="7">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0.39930555555555558</v>
+      </c>
       <c r="G30" s="7">
         <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
-        <v>0</v>
+        <v>4.5138888888888895E-2</v>
       </c>
       <c r="H30" s="7"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="5"/>
+      <c r="A31" s="3">
+        <v>45425</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D31" s="6"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="E31" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0.43055555555555558</v>
+      </c>
       <c r="G31" s="7">
         <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
-        <v>0</v>
+        <v>2.0833333333333315E-2</v>
       </c>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="5"/>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>45425</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="D32" s="6"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="E32" s="7">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="F32" s="7">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="G32" s="7">
         <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
-        <v>0</v>
+        <v>2.7777777777777735E-2</v>
       </c>
       <c r="H32" s="7"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="5"/>
+      <c r="A33" s="3">
+        <v>45425</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="E33" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F33" s="7">
+        <v>0.4826388888888889</v>
+      </c>
       <c r="G33" s="7">
         <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
-        <v>0</v>
+        <v>2.430555555555558E-2</v>
       </c>
       <c r="H33" s="7"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="5"/>
+      <c r="A34" s="3">
+        <v>45425</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="D34" s="6"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="E34" s="7">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="F34" s="7">
+        <v>0.51041666666666663</v>
+      </c>
       <c r="G34" s="7">
         <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
-        <v>0</v>
+        <v>2.7777777777777735E-2</v>
       </c>
       <c r="H34" s="7"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="5"/>
+      <c r="A35" s="3">
+        <v>45425</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="D35" s="6"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="E35" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0.59375</v>
+      </c>
       <c r="G35" s="7">
         <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
+      <c r="A36" s="3">
+        <v>45425</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0.59375</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="G36" s="7">
         <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
-        <v>0</v>
+        <v>3.472222222222221E-2</v>
       </c>
       <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+      <c r="A37" s="3">
+        <v>45426</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F37" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="G37" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="H37" s="7"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="A38" s="3">
+        <v>45426</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="F38" s="7">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="G38" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="H38" s="7"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+      <c r="A39" s="3">
+        <v>45426</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="F39" s="7">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="G39" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="H39" s="7"/>
+    </row>
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>45426</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="F40" s="7">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="G40" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="H40" s="7"/>
+    </row>
+    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>45426</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="F41" s="7">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="G41" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="H41" s="7"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
+      <c r="A42" s="3">
+        <v>45426</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="6"/>
+      <c r="E42" s="7">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="F42" s="7">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="G42" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="H42" s="7"/>
+    </row>
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>45426</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="7">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="F43" s="7">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="G43" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="H43" s="7"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+      <c r="A44" s="3">
+        <v>45426</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" s="7">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F44" s="7">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="G44" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>4.513888888888884E-2</v>
+      </c>
+      <c r="H44" s="7"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C45" s="2"/>
@@ -1766,9 +2085,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1886,25 +2208,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{213C64E1-87E2-4C8E-8457-B15D2DEDA5D9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC60CD4A-9E4F-42F0-BE26-5B273C83DB90}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1926,9 +2238,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC60CD4A-9E4F-42F0-BE26-5B273C83DB90}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{213C64E1-87E2-4C8E-8457-B15D2DEDA5D9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mise a jour de la documentation finale
Dernier commit pour ce projet tpi
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail_VMW.xlsx
+++ b/Documentation/Journal_de_travail_VMW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pt63nch\Documents\GitHub\Oublie pas\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E640FDBF-6620-47EE-862B-C9390D8D68E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26505A3-1302-4755-A34C-B49BC522B778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C76477CB-AF63-4402-801C-627B6AD4564C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="108">
   <si>
     <t>Date</t>
   </si>
@@ -292,6 +292,72 @@
   </si>
   <si>
     <t>Création de la base de donnée Room</t>
+  </si>
+  <si>
+    <t>Ajout d'une classe de préférence afin de stocker les tags</t>
+  </si>
+  <si>
+    <t>Création d'objectif</t>
+  </si>
+  <si>
+    <t>Affichage des tags</t>
+  </si>
+  <si>
+    <t>Affichage des objectif</t>
+  </si>
+  <si>
+    <t>La base de donnée a été mise a jour (version 3)</t>
+  </si>
+  <si>
+    <t>Changement de couleur de police</t>
+  </si>
+  <si>
+    <t>Ajout de statut</t>
+  </si>
+  <si>
+    <t>Classes mises a jours</t>
+  </si>
+  <si>
+    <t>Résolution de bug avec mes variables TimeMillis</t>
+  </si>
+  <si>
+    <t>Rédaction  de  commentaire, correction de bug mineurs</t>
+  </si>
+  <si>
+    <t>Ajout de la fonction d'annuler un objectif</t>
+  </si>
+  <si>
+    <t>Dernier commit d'implementation, correction de bug mineur</t>
+  </si>
+  <si>
+    <t>Documentation de la création de la base donnée</t>
+  </si>
+  <si>
+    <t>Documentation de l'implementation</t>
+  </si>
+  <si>
+    <t>Ajout d’un objectif dans la base de données , Affichage des objectifs, Ajout de statut</t>
+  </si>
+  <si>
+    <t>Modification d’un objectif, Tri de l’affichage des objectifs, Annulation d’une notification</t>
+  </si>
+  <si>
+    <t>Journal de travail et pdf mis a jour</t>
+  </si>
+  <si>
+    <t>uploadé sur github</t>
+  </si>
+  <si>
+    <t>Finalisation du dossier de projet</t>
+  </si>
+  <si>
+    <t>Push d'un patch qui corrige trois bug mineur</t>
+  </si>
+  <si>
+    <t>découvert lors de la phase de test</t>
+  </si>
+  <si>
+    <t>Préparation et rendu du TPI</t>
   </si>
 </sst>
 </file>
@@ -451,8 +517,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}" name="Tableau1" displayName="Tableau1" ref="A1:H59" totalsRowShown="0" dataDxfId="8">
-  <autoFilter ref="A1:H59" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}" name="Tableau1" displayName="Tableau1" ref="A1:H80" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="A1:H80" xr:uid="{E93C6E1C-B0BD-4EF6-B435-0E3DCB4B182F}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{F03BD8AE-DCAD-435E-AC03-584E15FC8493}" name="Date" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{76FA6963-7F8C-4895-B8BA-445A4BB2DC8E}" name="Type de travail" dataDxfId="6"/>
@@ -766,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA4812EB-3ED2-43D9-9F10-833A2D245EB4}">
-  <dimension ref="A1:I118"/>
+  <dimension ref="A1:I125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,7 +903,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="10">
         <f>SUM(G:G)</f>
-        <v>2.6597222222222223</v>
+        <v>3.7013888888888902</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2197,89 +2263,496 @@
       </c>
       <c r="H59" s="7"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
+    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>45435</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D60" s="6"/>
+      <c r="E60" s="7">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="F60" s="7">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="G60" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H60" s="7"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+      <c r="A61" s="3">
+        <v>45435</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D61" s="5"/>
+      <c r="E61" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="F61" s="7">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="G61" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>9.3749999999999944E-2</v>
+      </c>
+      <c r="H61" s="7"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
+      <c r="A62" s="3">
+        <v>45435</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62" s="5"/>
+      <c r="E62" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="F62" s="7">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G62" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="H62" s="7"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
+      <c r="A63" s="3">
+        <v>45435</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D63" s="5"/>
+      <c r="E63" s="7">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F63" s="7">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="G63" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="H63" s="7"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-    </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-    </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-    </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-    </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
+      <c r="A64" s="3">
+        <v>45435</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D64" s="5"/>
+      <c r="E64" s="7">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="F64" s="7">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="G64" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
+        <v>45436</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D65" s="6"/>
+      <c r="E65" s="7">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="F65" s="7">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="G65" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H65" s="7"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>45436</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D66" s="6"/>
+      <c r="E66" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="F66" s="7">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="G66" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>9.3749999999999944E-2</v>
+      </c>
+      <c r="H66" s="7"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>45436</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D67" s="6"/>
+      <c r="E67" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="F67" s="7">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G67" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="H67" s="7"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
+        <v>45436</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D68" s="6"/>
+      <c r="E68" s="7">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F68" s="7">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="G68" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="H68" s="7"/>
+    </row>
+    <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
+        <v>45436</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D69" s="6"/>
+      <c r="E69" s="7">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="F69" s="7">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="G69" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="H69" s="7"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <v>45439</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D70" s="6"/>
+      <c r="E70" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="F70" s="7">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="G70" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="H70" s="7"/>
+    </row>
+    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <v>45440</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D71" s="6"/>
+      <c r="E71" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F71" s="7">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="G71" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>6.5972222222222265E-2</v>
+      </c>
+      <c r="H71" s="7"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <v>45440</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D72" s="6"/>
+      <c r="E72" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="F72" s="7">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="G72" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>9.3749999999999944E-2</v>
+      </c>
+      <c r="H72" s="7"/>
+    </row>
+    <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <v>45440</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E73" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="F73" s="7">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G73" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="H73" s="7"/>
+    </row>
+    <row r="74" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
+        <v>45440</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E74" s="7">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F74" s="7">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="G74" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>2.430555555555558E-2</v>
+      </c>
+      <c r="H74" s="7"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
+        <v>45440</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E75" s="7">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="F75" s="7">
+        <v>0.70486111111111116</v>
+      </c>
+      <c r="G75" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="H75" s="7"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <v>45442</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D76" s="6"/>
+      <c r="E76" s="7">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="F76" s="7">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="G76" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="H76" s="7"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
+        <v>45442</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D77" s="6"/>
+      <c r="E77" s="7">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="F77" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G77" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>4.8611111111111049E-2</v>
+      </c>
+      <c r="H77" s="7"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <v>45442</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E78" s="7">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F78" s="7">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="G78" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="H78" s="7"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <v>45442</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D79" s="6"/>
+      <c r="E79" s="7">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F79" s="7">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="G79" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>3.1249999999999944E-2</v>
+      </c>
+      <c r="H79" s="7"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="3">
+        <v>45442</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80" s="6"/>
+      <c r="E80" s="7">
+        <v>0.5625</v>
+      </c>
+      <c r="F80" s="7">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="G80" s="7">
+        <f>SUM(Tableau1[[#This Row],[Heure de fin]]-Tableau1[[#This Row],[heure de début2]])</f>
+        <v>3.819444444444442E-2</v>
+      </c>
+      <c r="H80" s="7"/>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C81" s="2"/>
@@ -2433,10 +2906,38 @@
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
     </row>
+    <row r="119" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C119" s="2"/>
+      <c r="D119" s="2"/>
+    </row>
+    <row r="120" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C120" s="2"/>
+      <c r="D120" s="2"/>
+    </row>
+    <row r="121" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C121" s="2"/>
+      <c r="D121" s="2"/>
+    </row>
+    <row r="122" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
+    </row>
+    <row r="123" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
+    </row>
+    <row r="124" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C124" s="2"/>
+      <c r="D124" s="2"/>
+    </row>
+    <row r="125" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C125" s="2"/>
+      <c r="D125" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="80" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="60" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -2444,9 +2945,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2564,25 +3068,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{213C64E1-87E2-4C8E-8457-B15D2DEDA5D9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC60CD4A-9E4F-42F0-BE26-5B273C83DB90}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2604,9 +3098,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC60CD4A-9E4F-42F0-BE26-5B273C83DB90}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{213C64E1-87E2-4C8E-8457-B15D2DEDA5D9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>